<commit_message>
ST to Dh constraints fixed
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_new_model_basic.xlsx
+++ b/src/pv_optimizer_contracting/data_input_new_model_basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35484887-68E6-4ED5-AD5E-D4E266D1E0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47E58F9-5B73-4DEC-BDC6-C55FE960F841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6F6BA0A-853F-4A52-83CB-1D40EBCA633B}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1485,7 +1485,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1838,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429933C5-DFD0-42DC-9288-AD78420EFB5D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>